<commit_message>
Updated Color and Format
</commit_message>
<xml_diff>
--- a/ProjectWorkflowPhase1.xlsx
+++ b/ProjectWorkflowPhase1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,12 +356,16 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -373,12 +377,16 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -390,12 +398,16 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:pattFill prst="wdUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -466,7 +478,7 @@
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.0</c:v>
@@ -500,11 +512,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1774731680"/>
-        <c:axId val="1774733728"/>
+        <c:axId val="1615663376"/>
+        <c:axId val="1825253488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1774731680"/>
+        <c:axId val="1615663376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1774733728"/>
+        <c:crossAx val="1825253488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -611,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1774733728"/>
+        <c:axId val="1825253488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42770.0"/>
@@ -720,7 +732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1774731680"/>
+        <c:crossAx val="1615663376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1616,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1694,7 +1706,7 @@
         <v>42760</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>